<commit_message>
reflecting changes on header
</commit_message>
<xml_diff>
--- a/test/data/persons.xlsx
+++ b/test/data/persons.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Nome</t>
   </si>
@@ -25,9 +25,6 @@
     <t>Cargo</t>
   </si>
   <si>
-    <t>Telefones</t>
-  </si>
-  <si>
     <t>Endereço</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>552199401-1944,1234</t>
   </si>
   <si>
-    <t>Emails</t>
-  </si>
-  <si>
     <t xml:space="preserve">Carlos Alberto B.Tessarollo </t>
   </si>
   <si>
@@ -98,6 +92,15 @@
   </si>
   <si>
     <t>2354-4025</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
+    <t>E-mail</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -497,7 +500,7 @@
     <col min="5" max="5" width="49.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,92 +511,95 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>